<commit_message>
set up sensi analysis in source models; reorganized folder structure
sensi inputs are in last tab of sensi inputs spreadsheet
</commit_message>
<xml_diff>
--- a/Model/Sensi Runs/Master_160104/import.xlsx
+++ b/Model/Sensi Runs/Master_160104/import.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Peterson\GitHub\Utility-D-S\Model\Sensi Runs\Master_160104\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LA" sheetId="1" r:id="rId1"/>
@@ -13,8 +18,9 @@
     <sheet name="sensitivity" sheetId="3" r:id="rId4"/>
     <sheet name="all_variables" sheetId="2" r:id="rId5"/>
     <sheet name="Demand Charge" sheetId="6" r:id="rId6"/>
+    <sheet name="revised Sensi Setup" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +35,7 @@
     <author>Nick Laws</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -177,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -204,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -230,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -258,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -285,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -313,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="W1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -340,7 +346,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -364,7 +370,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -388,7 +394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -415,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -439,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0">
+    <comment ref="N2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -481,7 +487,7 @@
     <author>Nick Laws</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -505,7 +511,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -529,7 +535,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -553,7 +559,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -653,7 +659,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -680,7 +686,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -706,7 +712,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -734,7 +740,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -761,7 +767,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -789,7 +795,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="W1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -816,7 +822,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -840,7 +846,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -864,7 +870,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -891,7 +897,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -915,7 +921,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0">
+    <comment ref="N2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -957,7 +963,7 @@
     <author>Nick Laws</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -981,7 +987,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1016,7 +1022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1040,7 +1046,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1064,7 +1070,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1164,7 +1170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1191,7 +1197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1217,7 +1223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1245,7 +1251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1272,7 +1278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1300,7 +1306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="W1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1327,7 +1333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1351,7 +1357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1375,7 +1381,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1402,7 +1408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1427,7 +1433,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0">
+    <comment ref="N2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1459,7 +1465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA2" authorId="0">
+    <comment ref="AA2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1493,7 +1499,7 @@
     <author>Nick Laws</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1593,7 +1599,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1693,7 +1699,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1722,7 +1728,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="192">
   <si>
     <t>population growth rate</t>
   </si>
@@ -2238,12 +2244,72 @@
   </si>
   <si>
     <t>(estimated)</t>
+  </si>
+  <si>
+    <t>PV_incentive</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>5,</t>
+  </si>
+  <si>
+    <t>Battery_incentive</t>
+  </si>
+  <si>
+    <t>InnovationScaleFactor</t>
+  </si>
+  <si>
+    <t>ImitationScaleFactor</t>
+  </si>
+  <si>
+    <t>use_limit_on_ratio_of_PV_to_total_hhold</t>
+  </si>
+  <si>
+    <t>efficiency_improvement_of_reg_customers_as_%_per_year</t>
+  </si>
+  <si>
+    <t>util_fixed_cost_growth_rate_%_per_year</t>
+  </si>
+  <si>
+    <t>wholesale_price_growth_rate_%_per_year</t>
+  </si>
+  <si>
+    <t>debt_interest_rate_as_%</t>
+  </si>
+  <si>
+    <t>Equity_Fraction</t>
+  </si>
+  <si>
+    <t>Req'd_Rate_of_Return_as_%</t>
+  </si>
+  <si>
+    <t>0, 5000</t>
+  </si>
+  <si>
+    <t>1, 5</t>
+  </si>
+  <si>
+    <t>0.01, 0.05</t>
+  </si>
+  <si>
+    <t>1,0</t>
+  </si>
+  <si>
+    <t>1, 10</t>
+  </si>
+  <si>
+    <t>0.5, 2</t>
+  </si>
+  <si>
+    <t>0.1, 0.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -3140,27 +3206,27 @@
       <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="9" max="9" width="11.875" customWidth="1"/>
+    <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" style="48"/>
-    <col min="17" max="17" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="11" style="35"/>
-    <col min="26" max="26" width="15.33203125" customWidth="1"/>
-    <col min="49" max="49" width="14.6640625" customWidth="1"/>
-    <col min="108" max="108" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.375" customWidth="1"/>
+    <col min="49" max="49" width="14.625" customWidth="1"/>
+    <col min="108" max="108" width="11.875" bestFit="1" customWidth="1"/>
     <col min="122" max="122" width="15" customWidth="1"/>
-    <col min="132" max="132" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="143" max="144" width="13.33203125" customWidth="1"/>
-    <col min="146" max="146" width="13.6640625" customWidth="1"/>
+    <col min="132" max="132" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="143" max="144" width="13.375" customWidth="1"/>
+    <col min="146" max="146" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="14" customFormat="1" ht="64" customHeight="1">
+    <row r="1" spans="1:27" s="14" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="14" t="s">
         <v>7</v>
       </c>
@@ -3240,7 +3306,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="32" customFormat="1">
+    <row r="2" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>150</v>
       </c>
@@ -3323,7 +3389,7 @@
         <v>6211.2916123429659</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="9" customFormat="1">
+    <row r="3" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3384,7 +3450,7 @@
         <v>1.12380952380952</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="9" customFormat="1">
+    <row r="4" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -3445,7 +3511,7 @@
         <v>1.2253968253968299</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="9" customFormat="1">
+    <row r="5" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -3506,7 +3572,7 @@
         <v>1.35238095238095</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
@@ -3567,7 +3633,7 @@
         <v>1.4539682539682499</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="4" customFormat="1">
+    <row r="7" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -3629,7 +3695,7 @@
         <v>1.5492063492063499</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J8" s="23">
         <v>5.0739549839228298E-3</v>
       </c>
@@ -3682,7 +3748,7 @@
         <v>1.6317460317460299</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>155</v>
       </c>
@@ -3738,7 +3804,7 @@
         <v>1.6952380952381001</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J10" s="23">
         <v>4.1093247588424404E-3</v>
       </c>
@@ -3791,7 +3857,7 @@
         <v>1.7904761904761901</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J11" s="23">
         <v>3.6077170418006401E-3</v>
       </c>
@@ -3844,7 +3910,7 @@
         <v>1.89206349206349</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J12" s="23">
         <v>2.9710610932475899E-3</v>
       </c>
@@ -3897,7 +3963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="K13" s="48">
         <v>12700</v>
       </c>
@@ -3929,7 +3995,7 @@
         <v>0.42399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -3965,7 +4031,7 @@
         <v>0.41199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="C15" s="12"/>
       <c r="F15" s="12"/>
@@ -4000,7 +4066,7 @@
         <v>0.39900000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="K16" s="48">
         <v>12245</v>
       </c>
@@ -4032,7 +4098,7 @@
         <v>0.38700000000000001</v>
       </c>
     </row>
-    <row r="17" spans="11:25">
+    <row r="17" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K17" s="48">
         <v>12155</v>
       </c>
@@ -4064,7 +4130,7 @@
         <v>0.379</v>
       </c>
     </row>
-    <row r="18" spans="11:25">
+    <row r="18" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K18" s="48">
         <v>12065</v>
       </c>
@@ -4096,7 +4162,7 @@
         <v>0.379</v>
       </c>
     </row>
-    <row r="19" spans="11:25">
+    <row r="19" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K19" s="48">
         <v>11975</v>
       </c>
@@ -4128,7 +4194,7 @@
         <v>0.372</v>
       </c>
     </row>
-    <row r="20" spans="11:25">
+    <row r="20" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K20" s="48">
         <v>11900</v>
       </c>
@@ -4160,7 +4226,7 @@
         <v>0.371</v>
       </c>
     </row>
-    <row r="21" spans="11:25">
+    <row r="21" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K21" s="48">
         <v>11795</v>
       </c>
@@ -4192,7 +4258,7 @@
         <v>0.36699999999999999</v>
       </c>
     </row>
-    <row r="22" spans="11:25">
+    <row r="22" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K22" s="48">
         <v>11550</v>
       </c>
@@ -4224,7 +4290,7 @@
         <v>0.36399999999999999</v>
       </c>
     </row>
-    <row r="23" spans="11:25">
+    <row r="23" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K23" s="48">
         <v>11435</v>
       </c>
@@ -4250,7 +4316,7 @@
         <v>0.36199999999999999</v>
       </c>
     </row>
-    <row r="24" spans="11:25">
+    <row r="24" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K24" s="48">
         <v>11400</v>
       </c>
@@ -4276,7 +4342,7 @@
         <v>0.36099999999999999</v>
       </c>
     </row>
-    <row r="25" spans="11:25">
+    <row r="25" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K25" s="48">
         <v>11380</v>
       </c>
@@ -4302,7 +4368,7 @@
         <v>0.35899999999999999</v>
       </c>
     </row>
-    <row r="26" spans="11:25">
+    <row r="26" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K26" s="48">
         <v>11360</v>
       </c>
@@ -4328,7 +4394,7 @@
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="27" spans="11:25">
+    <row r="27" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K27" s="48">
         <v>11340</v>
       </c>
@@ -4354,7 +4420,7 @@
         <v>0.35499999999999998</v>
       </c>
     </row>
-    <row r="28" spans="11:25">
+    <row r="28" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K28" s="48">
         <v>11320</v>
       </c>
@@ -4380,7 +4446,7 @@
         <v>0.35299999999999998</v>
       </c>
     </row>
-    <row r="29" spans="11:25">
+    <row r="29" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K29" s="48">
         <v>11300</v>
       </c>
@@ -4406,7 +4472,7 @@
         <v>0.35099999999999998</v>
       </c>
     </row>
-    <row r="30" spans="11:25">
+    <row r="30" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K30" s="48">
         <v>11280</v>
       </c>
@@ -4432,7 +4498,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="31" spans="11:25">
+    <row r="31" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K31" s="48">
         <v>11260</v>
       </c>
@@ -4458,7 +4524,7 @@
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="32" spans="11:25">
+    <row r="32" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K32" s="48">
         <v>11240</v>
       </c>
@@ -4484,7 +4550,7 @@
         <v>0.34599999999999997</v>
       </c>
     </row>
-    <row r="33" spans="11:25">
+    <row r="33" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K33" s="48">
         <v>11220</v>
       </c>
@@ -4510,7 +4576,7 @@
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="34" spans="11:25">
+    <row r="34" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K34" s="48">
         <v>11200</v>
       </c>
@@ -4536,7 +4602,7 @@
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="35" spans="11:25">
+    <row r="35" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K35" s="48">
         <v>11180</v>
       </c>
@@ -4562,7 +4628,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="36" spans="11:25">
+    <row r="36" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K36" s="48">
         <v>11160</v>
       </c>
@@ -4588,7 +4654,7 @@
         <v>0.33900000000000002</v>
       </c>
     </row>
-    <row r="37" spans="11:25">
+    <row r="37" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K37" s="48">
         <v>11140</v>
       </c>
@@ -4614,7 +4680,7 @@
         <v>0.33800000000000002</v>
       </c>
     </row>
-    <row r="38" spans="11:25">
+    <row r="38" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K38" s="48">
         <v>11120</v>
       </c>
@@ -4654,27 +4720,27 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.625" customWidth="1"/>
+    <col min="17" max="17" width="13.875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.33203125" customWidth="1"/>
-    <col min="49" max="49" width="14.6640625" customWidth="1"/>
-    <col min="108" max="108" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.375" customWidth="1"/>
+    <col min="49" max="49" width="14.625" customWidth="1"/>
+    <col min="108" max="108" width="11.875" bestFit="1" customWidth="1"/>
     <col min="122" max="122" width="15" customWidth="1"/>
-    <col min="132" max="132" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="143" max="144" width="13.33203125" customWidth="1"/>
-    <col min="146" max="146" width="13.6640625" customWidth="1"/>
+    <col min="132" max="132" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="143" max="144" width="13.375" customWidth="1"/>
+    <col min="146" max="146" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="15" customFormat="1" ht="64" customHeight="1">
+    <row r="1" spans="1:27" s="15" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
         <v>7</v>
       </c>
@@ -4754,7 +4820,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="32" customFormat="1">
+    <row r="2" spans="1:27" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>150</v>
       </c>
@@ -4837,7 +4903,7 @@
         <v>7007.1402678343975</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="9" customFormat="1">
+    <row r="3" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -4898,7 +4964,7 @@
         <v>1.12380952380952</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="9" customFormat="1">
+    <row r="4" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -4959,7 +5025,7 @@
         <v>1.2253968253968299</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="9" customFormat="1">
+    <row r="5" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -5020,7 +5086,7 @@
         <v>1.35238095238095</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
@@ -5081,7 +5147,7 @@
         <v>1.4539682539682499</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="4" customFormat="1">
+    <row r="7" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -5143,7 +5209,7 @@
         <v>1.5492063492063499</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J8" s="23">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -5196,7 +5262,7 @@
         <v>1.6317460317460299</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
         <v>161</v>
       </c>
@@ -5252,7 +5318,7 @@
         <v>1.6952380952381001</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J10" s="23">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -5305,7 +5371,7 @@
         <v>1.7904761904761901</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J11" s="23">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -5358,7 +5424,7 @@
         <v>1.89206349206349</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="J12" s="23">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -5411,7 +5477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="K13" s="48">
         <v>23622</v>
       </c>
@@ -5443,7 +5509,7 @@
         <v>0.42399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -5479,7 +5545,7 @@
         <v>0.41199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="C15" s="12"/>
       <c r="F15" s="12"/>
@@ -5514,7 +5580,7 @@
         <v>0.39900000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="K16" s="48">
         <v>22775.7</v>
       </c>
@@ -5546,7 +5612,7 @@
         <v>0.38700000000000001</v>
       </c>
     </row>
-    <row r="17" spans="11:25">
+    <row r="17" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K17" s="48">
         <v>22608.300000000003</v>
       </c>
@@ -5578,7 +5644,7 @@
         <v>0.379</v>
       </c>
     </row>
-    <row r="18" spans="11:25">
+    <row r="18" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K18" s="48">
         <v>22440.9</v>
       </c>
@@ -5610,7 +5676,7 @@
         <v>0.379</v>
       </c>
     </row>
-    <row r="19" spans="11:25">
+    <row r="19" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K19" s="48">
         <v>22273.5</v>
       </c>
@@ -5642,7 +5708,7 @@
         <v>0.372</v>
       </c>
     </row>
-    <row r="20" spans="11:25">
+    <row r="20" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K20" s="48">
         <v>22134</v>
       </c>
@@ -5674,7 +5740,7 @@
         <v>0.371</v>
       </c>
     </row>
-    <row r="21" spans="11:25">
+    <row r="21" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K21" s="48">
         <v>21938.7</v>
       </c>
@@ -5706,7 +5772,7 @@
         <v>0.36699999999999999</v>
       </c>
     </row>
-    <row r="22" spans="11:25">
+    <row r="22" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K22" s="48">
         <v>21483</v>
       </c>
@@ -5738,7 +5804,7 @@
         <v>0.36399999999999999</v>
       </c>
     </row>
-    <row r="23" spans="11:25">
+    <row r="23" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K23" s="48">
         <v>21269.100000000002</v>
       </c>
@@ -5764,7 +5830,7 @@
         <v>0.36199999999999999</v>
       </c>
     </row>
-    <row r="24" spans="11:25">
+    <row r="24" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K24" s="48">
         <v>21204</v>
       </c>
@@ -5790,7 +5856,7 @@
         <v>0.36099999999999999</v>
       </c>
     </row>
-    <row r="25" spans="11:25">
+    <row r="25" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K25" s="48">
         <v>21166.800000000003</v>
       </c>
@@ -5816,7 +5882,7 @@
         <v>0.35899999999999999</v>
       </c>
     </row>
-    <row r="26" spans="11:25">
+    <row r="26" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K26" s="48">
         <v>21129.600000000002</v>
       </c>
@@ -5842,7 +5908,7 @@
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="27" spans="11:25">
+    <row r="27" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K27" s="48">
         <v>21092.400000000001</v>
       </c>
@@ -5868,7 +5934,7 @@
         <v>0.35499999999999998</v>
       </c>
     </row>
-    <row r="28" spans="11:25">
+    <row r="28" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K28" s="48">
         <v>21055.200000000001</v>
       </c>
@@ -5894,7 +5960,7 @@
         <v>0.35299999999999998</v>
       </c>
     </row>
-    <row r="29" spans="11:25">
+    <row r="29" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K29" s="48">
         <v>21018</v>
       </c>
@@ -5920,7 +5986,7 @@
         <v>0.35099999999999998</v>
       </c>
     </row>
-    <row r="30" spans="11:25">
+    <row r="30" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K30" s="48">
         <v>20980.800000000003</v>
       </c>
@@ -5946,7 +6012,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="31" spans="11:25">
+    <row r="31" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K31" s="48">
         <v>20943.600000000002</v>
       </c>
@@ -5972,7 +6038,7 @@
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="32" spans="11:25">
+    <row r="32" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K32" s="48">
         <v>20906.400000000001</v>
       </c>
@@ -5998,7 +6064,7 @@
         <v>0.34599999999999997</v>
       </c>
     </row>
-    <row r="33" spans="11:25">
+    <row r="33" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K33" s="48">
         <v>20869.2</v>
       </c>
@@ -6024,7 +6090,7 @@
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="34" spans="11:25">
+    <row r="34" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K34" s="48">
         <v>20832</v>
       </c>
@@ -6050,7 +6116,7 @@
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="35" spans="11:25">
+    <row r="35" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K35" s="48">
         <v>20794.800000000003</v>
       </c>
@@ -6076,7 +6142,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="36" spans="11:25">
+    <row r="36" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K36" s="48">
         <v>20757.600000000002</v>
       </c>
@@ -6102,7 +6168,7 @@
         <v>0.33900000000000002</v>
       </c>
     </row>
-    <row r="37" spans="11:25">
+    <row r="37" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K37" s="48">
         <v>20720.400000000001</v>
       </c>
@@ -6128,7 +6194,7 @@
         <v>0.33800000000000002</v>
       </c>
     </row>
-    <row r="38" spans="11:25">
+    <row r="38" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K38" s="48">
         <v>20683.2</v>
       </c>
@@ -6164,13 +6230,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="AB22" sqref="AB22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:29" s="15" customFormat="1" ht="64" customHeight="1">
+    <row r="1" spans="1:29" s="15" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
         <v>7</v>
       </c>
@@ -6250,7 +6316,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="15" customFormat="1" ht="18" customHeight="1">
+    <row r="2" spans="1:29" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1448848</v>
       </c>
@@ -6333,7 +6399,7 @@
       <c r="AB2"/>
       <c r="AC2"/>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="I3" s="59"/>
       <c r="J3" s="60">
         <v>1.7999999999999999E-2</v>
@@ -6387,7 +6453,7 @@
         <v>1.12380952380952</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J4" s="60">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -6440,7 +6506,7 @@
         <v>1.2253968253968299</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J5" s="60">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -6493,7 +6559,7 @@
         <v>1.35238095238095</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J6" s="60">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -6546,7 +6612,7 @@
         <v>1.4539682539682499</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
         <v>161</v>
       </c>
@@ -6602,7 +6668,7 @@
         <v>1.5492063492063499</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J8" s="60">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -6655,7 +6721,7 @@
         <v>1.6317460317460299</v>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J9" s="60">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -6708,7 +6774,7 @@
         <v>1.6952380952381001</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J10" s="60">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -6761,7 +6827,7 @@
         <v>1.7904761904761901</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J11" s="60">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -6814,7 +6880,7 @@
         <v>1.89206349206349</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J12" s="60">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -6867,7 +6933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K13" s="58">
         <v>7201.1257841214756</v>
       </c>
@@ -6899,7 +6965,7 @@
         <v>0.42399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K14" s="58">
         <v>7064.304394223167</v>
       </c>
@@ -6931,7 +6997,7 @@
         <v>0.41199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K15" s="58">
         <v>6930.0826107329258</v>
       </c>
@@ -6963,7 +7029,7 @@
         <v>0.39900000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K16" s="58">
         <v>6798.4110411290003</v>
       </c>
@@ -6995,7 +7061,7 @@
         <v>0.38700000000000001</v>
       </c>
     </row>
-    <row r="17" spans="11:25">
+    <row r="17" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K17" s="58">
         <v>6669.2412313475497</v>
       </c>
@@ -7027,7 +7093,7 @@
         <v>0.379</v>
       </c>
     </row>
-    <row r="18" spans="11:25">
+    <row r="18" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K18" s="58">
         <v>6542.5256479519448</v>
       </c>
@@ -7059,7 +7125,7 @@
         <v>0.379</v>
       </c>
     </row>
-    <row r="19" spans="11:25">
+    <row r="19" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K19" s="58">
         <v>6418.2176606408584</v>
       </c>
@@ -7091,7 +7157,7 @@
         <v>0.372</v>
       </c>
     </row>
-    <row r="20" spans="11:25">
+    <row r="20" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K20" s="58">
         <v>6296.2715250886813</v>
       </c>
@@ -7123,7 +7189,7 @@
         <v>0.371</v>
       </c>
     </row>
-    <row r="21" spans="11:25">
+    <row r="21" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K21" s="58">
         <v>6176.6423661119961</v>
       </c>
@@ -7155,7 +7221,7 @@
         <v>0.36699999999999999</v>
       </c>
     </row>
-    <row r="22" spans="11:25">
+    <row r="22" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K22" s="58">
         <v>6059.2861611558683</v>
       </c>
@@ -7187,7 +7253,7 @@
         <v>0.36399999999999999</v>
       </c>
     </row>
-    <row r="23" spans="11:25">
+    <row r="23" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K23" s="58">
         <v>5944.1597240939063</v>
       </c>
@@ -7213,7 +7279,7 @@
         <v>0.36199999999999999</v>
       </c>
     </row>
-    <row r="24" spans="11:25">
+    <row r="24" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K24" s="58">
         <v>5831.2206893361217</v>
       </c>
@@ -7239,7 +7305,7 @@
         <v>0.36099999999999999</v>
       </c>
     </row>
-    <row r="25" spans="11:25">
+    <row r="25" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K25" s="58">
         <v>5720.4274962387353</v>
       </c>
@@ -7265,7 +7331,7 @@
         <v>0.35899999999999999</v>
       </c>
     </row>
-    <row r="26" spans="11:25">
+    <row r="26" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K26" s="58">
         <v>5611.7393738102</v>
       </c>
@@ -7291,7 +7357,7 @@
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="27" spans="11:25">
+    <row r="27" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K27" s="58">
         <v>5505.1163257078051</v>
       </c>
@@ -7317,7 +7383,7 @@
         <v>0.35499999999999998</v>
       </c>
     </row>
-    <row r="28" spans="11:25">
+    <row r="28" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K28" s="58">
         <v>5400.5191155193561</v>
       </c>
@@ -7343,7 +7409,7 @@
         <v>0.35299999999999998</v>
       </c>
     </row>
-    <row r="29" spans="11:25">
+    <row r="29" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K29" s="58">
         <v>5297.909252324489</v>
       </c>
@@ -7369,7 +7435,7 @@
         <v>0.35099999999999998</v>
       </c>
     </row>
-    <row r="30" spans="11:25">
+    <row r="30" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K30" s="58">
         <v>5197.2489765303226</v>
       </c>
@@ -7395,7 +7461,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="31" spans="11:25">
+    <row r="31" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K31" s="58">
         <v>5098.5012459762474</v>
       </c>
@@ -7421,7 +7487,7 @@
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="32" spans="11:25">
+    <row r="32" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K32" s="58">
         <v>5001.6297223026977</v>
       </c>
@@ -7447,7 +7513,7 @@
         <v>0.34599999999999997</v>
       </c>
     </row>
-    <row r="33" spans="11:25">
+    <row r="33" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K33" s="58">
         <v>4906.5987575789477</v>
       </c>
@@ -7473,7 +7539,7 @@
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="34" spans="11:25">
+    <row r="34" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K34" s="58">
         <v>4813.373381184947</v>
       </c>
@@ -7499,7 +7565,7 @@
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="35" spans="11:25">
+    <row r="35" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K35" s="58">
         <v>4721.9192869424332</v>
       </c>
@@ -7525,7 +7591,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="36" spans="11:25">
+    <row r="36" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K36" s="58">
         <v>4632.2028204905273</v>
       </c>
@@ -7551,7 +7617,7 @@
         <v>0.33900000000000002</v>
       </c>
     </row>
-    <row r="37" spans="11:25">
+    <row r="37" spans="11:25" x14ac:dyDescent="0.25">
       <c r="K37" s="58">
         <v>4544.1909669012066</v>
       </c>
@@ -7577,7 +7643,7 @@
         <v>0.33800000000000002</v>
       </c>
     </row>
-    <row r="38" spans="11:25">
+    <row r="38" spans="11:25" x14ac:dyDescent="0.25">
       <c r="N38" s="17">
         <v>300</v>
       </c>
@@ -7602,21 +7668,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
     <col min="14" max="14" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="36" customFormat="1" ht="60">
+    <row r="1" spans="1:18" s="36" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B1" s="61" t="s">
         <v>113</v>
       </c>
@@ -7666,7 +7732,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="65" customFormat="1">
+    <row r="2" spans="1:18" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="36">
         <v>0</v>
@@ -7717,7 +7783,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>5000</v>
       </c>
@@ -7767,7 +7833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" s="13">
         <v>10000</v>
       </c>
@@ -7817,7 +7883,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="J5" s="73">
@@ -7829,7 +7895,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="J6" s="72">
@@ -7841,7 +7907,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J7" s="72">
         <v>0.95390070921985803</v>
       </c>
@@ -7851,7 +7917,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="J8" s="72">
@@ -7863,7 +7929,7 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>169</v>
       </c>
@@ -7874,7 +7940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J10" s="72">
         <v>0.83333333333333304</v>
       </c>
@@ -7882,7 +7948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="64"/>
       <c r="J11" s="72">
         <v>0.78723404255319196</v>
@@ -7890,8 +7956,26 @@
       <c r="K11" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="M11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>173</v>
+      </c>
+      <c r="P11" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>173</v>
+      </c>
+      <c r="R11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="57" t="s">
         <v>165</v>
       </c>
@@ -7902,7 +7986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>164</v>
       </c>
@@ -7913,7 +7997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="54" t="s">
         <v>163</v>
       </c>
@@ -7924,7 +8008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J15" s="72">
         <v>0.28723404255319201</v>
       </c>
@@ -7932,7 +8016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J16" s="72">
         <v>0.184397163120567</v>
       </c>
@@ -7940,7 +8024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="10:11">
+    <row r="17" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J17" s="72">
         <v>8.5106382978723402E-2</v>
       </c>
@@ -7948,7 +8032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="10:11">
+    <row r="18" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J18" s="72">
         <v>4.2553191489361701E-2</v>
       </c>
@@ -7956,7 +8040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="10:11">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J19" s="72">
         <v>2.1276595744680899E-2</v>
       </c>
@@ -7964,7 +8048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="10:11">
+    <row r="20" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J20" s="72">
         <v>3.54609929078014E-3</v>
       </c>
@@ -7972,7 +8056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="10:11">
+    <row r="21" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J21" s="72">
         <v>0</v>
       </c>
@@ -7980,7 +8064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="10:11">
+    <row r="22" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J22" s="72">
         <v>0</v>
       </c>
@@ -8008,16 +8092,16 @@
       <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:150" s="5" customFormat="1" ht="64" customHeight="1">
+    <row r="1" spans="1:150" s="5" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -8469,7 +8553,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:150">
+    <row r="7" spans="1:150" x14ac:dyDescent="0.25">
       <c r="T7" s="36" t="s">
         <v>162</v>
       </c>
@@ -8493,17 +8577,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>167</v>
       </c>
@@ -8511,7 +8595,7 @@
         <v>6211.2916123429659</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>168</v>
       </c>
@@ -8519,7 +8603,7 @@
         <v>7007.1402678343975</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>170</v>
       </c>
@@ -8539,4 +8623,119 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f>2^11</f>
+        <v>2048</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>